<commit_message>
Add new reserv people
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="145">
   <si>
     <t xml:space="preserve">Садатов Акбар Ариф огоы</t>
   </si>
@@ -416,6 +416,45 @@
   </si>
   <si>
     <t xml:space="preserve">@m_grek71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дулепа Милана Богдановна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Юрфак</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@mxllln</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Комарова Диана Алексеевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@wwsdiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Строкова Дарина Дмитриевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@darri_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лялюева Таисия Сергеевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@talymndas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Масленникова Светлана Евгеньевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@s_vv_et</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Самигуллина Зухра Ринатовна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@wqrexo</t>
   </si>
 </sst>
 </file>
@@ -523,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:D174"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1289,22 +1328,76 @@
       </c>
       <c r="D63" s="0"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="D64" s="0"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="D65" s="0"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="D66" s="0"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="D67" s="0"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="D68" s="0"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="D69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add all new reserv people
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="162">
   <si>
     <t xml:space="preserve">Садатов Акбар Ариф огоы</t>
   </si>
@@ -455,6 +455,57 @@
   </si>
   <si>
     <t xml:space="preserve">@wqrexo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Родионова Александра Владимировна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ИтиАБД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@tg_alessandra_rodionova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Бородин Никита Игоревич</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@call17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Логинов Максим Денисович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Python_abuser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Закревский Константин Сергеевич</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Rigel_125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Катлярова Самира Шавкатовна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@katmiraa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Зарубина Диана Евгеньевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@meowwow66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мамедова Мария Владимировна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@mashvixx1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Крылова Мария Григорьевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@mashkaklyger</t>
   </si>
 </sst>
 </file>
@@ -562,8 +613,8 @@
   </sheetPr>
   <dimension ref="A1:D174"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D73" activeCellId="0" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1400,28 +1451,100 @@
       </c>
       <c r="D69" s="0"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D70" s="0"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="D71" s="0"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="D72" s="0"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="D73" s="0"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="D74" s="0"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="D75" s="0"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="D76" s="0"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="D77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>